<commit_message>
JS functions t/m opdr7
</commit_message>
<xml_diff>
--- a/Clyde_softskills/OKR framework IrenevDijk Q1.xlsx
+++ b/Clyde_softskills/OKR framework IrenevDijk Q1.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/irene/Desktop/Techgrounds/NEW-TG-Web-development/Clyde_softskills/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E006978-447A-074A-BAFB-D0470955EADA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5214736-9B36-7B41-BB6B-F37BF83C02DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
   <si>
     <t>Timeframe</t>
   </si>
@@ -131,6 +132,9 @@
   </si>
   <si>
     <t>Atomic habits uitgelezen</t>
+  </si>
+  <si>
+    <t>mark manson uitgelezen</t>
   </si>
 </sst>
 </file>
@@ -453,13 +457,23 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="11" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -474,17 +488,7 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="10" fontId="11" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -706,7 +710,7 @@
   <dimension ref="A1:M1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -743,25 +747,25 @@
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="42"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="48"/>
       <c r="E2" s="6"/>
       <c r="F2" s="7"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="42"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="48"/>
       <c r="J2" s="8"/>
       <c r="K2" s="9"/>
       <c r="L2" s="10"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="45"/>
-      <c r="B3" s="46"/>
-      <c r="C3" s="47" t="s">
+      <c r="A3" s="51"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="44"/>
-      <c r="E3" s="42"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="48"/>
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
       <c r="H3" s="12"/>
@@ -782,11 +786,11 @@
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
       <c r="I4" s="14"/>
-      <c r="J4" s="48" t="s">
+      <c r="J4" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="37"/>
-      <c r="L4" s="37"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
@@ -795,16 +799,16 @@
       <c r="B5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
       <c r="F5" s="16"/>
-      <c r="G5" s="39" t="s">
+      <c r="G5" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="37"/>
+      <c r="H5" s="40"/>
       <c r="I5" s="15" t="s">
         <v>13</v>
       </c>
@@ -825,16 +829,16 @@
       <c r="B6" s="19">
         <v>1</v>
       </c>
-      <c r="C6" s="49" t="s">
+      <c r="C6" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
       <c r="F6" s="20">
-        <v>0.33</v>
-      </c>
-      <c r="G6" s="40"/>
-      <c r="H6" s="37"/>
+        <v>0.66</v>
+      </c>
+      <c r="G6" s="45"/>
+      <c r="H6" s="40"/>
       <c r="I6" s="21" t="s">
         <v>16</v>
       </c>
@@ -847,12 +851,12 @@
       <c r="B7" s="19">
         <v>2</v>
       </c>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
       <c r="F7" s="24"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="37"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="40"/>
       <c r="I7" s="25"/>
       <c r="J7" s="22"/>
       <c r="K7" s="23"/>
@@ -863,12 +867,12 @@
       <c r="B8" s="19">
         <v>3</v>
       </c>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
       <c r="F8" s="24"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="37"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="40"/>
       <c r="I8" s="25"/>
       <c r="J8" s="22"/>
       <c r="K8" s="23"/>
@@ -879,12 +883,12 @@
       <c r="B9" s="19">
         <v>4</v>
       </c>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
       <c r="F9" s="24"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="37"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="40"/>
       <c r="I9" s="25"/>
       <c r="J9" s="22"/>
       <c r="K9" s="23"/>
@@ -897,18 +901,18 @@
       <c r="B10" s="19">
         <v>5</v>
       </c>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
       <c r="F10" s="24"/>
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
-      <c r="J10" s="50" t="s">
+      <c r="J10" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="K10" s="37"/>
-      <c r="L10" s="37"/>
+      <c r="K10" s="40"/>
+      <c r="L10" s="40"/>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="28" t="s">
@@ -917,16 +921,16 @@
       <c r="B11" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
       <c r="F11" s="29"/>
-      <c r="G11" s="39" t="s">
+      <c r="G11" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="37"/>
+      <c r="H11" s="40"/>
       <c r="I11" s="15" t="s">
         <v>13</v>
       </c>
@@ -947,16 +951,16 @@
       <c r="B12" s="19">
         <v>1</v>
       </c>
-      <c r="C12" s="49" t="s">
+      <c r="C12" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
       <c r="F12" s="20">
         <v>0.1</v>
       </c>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
       <c r="I12" s="33" t="s">
         <v>20</v>
       </c>
@@ -969,16 +973,16 @@
       <c r="B13" s="19">
         <v>2</v>
       </c>
-      <c r="C13" s="49" t="s">
+      <c r="C13" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
       <c r="F13" s="20">
         <v>0.1</v>
       </c>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
       <c r="I13" s="33" t="s">
         <v>22</v>
       </c>
@@ -991,16 +995,16 @@
       <c r="B14" s="19">
         <v>3</v>
       </c>
-      <c r="C14" s="49" t="s">
+      <c r="C14" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
       <c r="F14" s="20">
         <v>0.08</v>
       </c>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
       <c r="I14" s="33" t="s">
         <v>24</v>
       </c>
@@ -1013,12 +1017,12 @@
       <c r="B15" s="19">
         <v>4</v>
       </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
       <c r="F15" s="24"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
       <c r="I15" s="25"/>
       <c r="J15" s="23"/>
       <c r="K15" s="23"/>
@@ -1029,12 +1033,12 @@
       <c r="B16" s="19">
         <v>5</v>
       </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
       <c r="F16" s="24"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
       <c r="I16" s="25"/>
       <c r="J16" s="23"/>
       <c r="K16" s="23"/>
@@ -1045,18 +1049,18 @@
       <c r="B17" s="3">
         <v>6</v>
       </c>
-      <c r="C17" s="51"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="52"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="44"/>
       <c r="F17" s="3"/>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
-      <c r="J17" s="48" t="s">
+      <c r="J17" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="K17" s="37"/>
-      <c r="L17" s="37"/>
+      <c r="K17" s="40"/>
+      <c r="L17" s="40"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
@@ -1065,16 +1069,16 @@
       <c r="B18" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="38" t="s">
+      <c r="C18" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
       <c r="F18" s="34"/>
-      <c r="G18" s="39" t="s">
+      <c r="G18" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="H18" s="37"/>
+      <c r="H18" s="40"/>
       <c r="I18" s="15" t="s">
         <v>13</v>
       </c>
@@ -1093,12 +1097,12 @@
       <c r="B19" s="19">
         <v>1</v>
       </c>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
       <c r="F19" s="24"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
       <c r="I19" s="25"/>
       <c r="J19" s="23"/>
       <c r="K19" s="23"/>
@@ -1109,12 +1113,12 @@
       <c r="B20" s="19">
         <v>2</v>
       </c>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
       <c r="F20" s="24"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="37"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
       <c r="I20" s="25"/>
       <c r="J20" s="23"/>
       <c r="K20" s="23"/>
@@ -1125,12 +1129,12 @@
       <c r="B21" s="19">
         <v>3</v>
       </c>
-      <c r="C21" s="37"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="37"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
       <c r="F21" s="24"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="37"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
       <c r="I21" s="25"/>
       <c r="J21" s="23"/>
       <c r="K21" s="23"/>
@@ -1141,12 +1145,12 @@
       <c r="B22" s="19">
         <v>4</v>
       </c>
-      <c r="C22" s="37"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="37"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
       <c r="F22" s="24"/>
-      <c r="G22" s="37"/>
-      <c r="H22" s="37"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
       <c r="I22" s="25"/>
       <c r="J22" s="23"/>
       <c r="K22" s="23"/>
@@ -1157,12 +1161,12 @@
       <c r="B23" s="19">
         <v>5</v>
       </c>
-      <c r="C23" s="37"/>
-      <c r="D23" s="37"/>
-      <c r="E23" s="37"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
       <c r="F23" s="24"/>
-      <c r="G23" s="37"/>
-      <c r="H23" s="37"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
       <c r="I23" s="25"/>
       <c r="J23" s="23"/>
       <c r="K23" s="23"/>
@@ -1173,9 +1177,9 @@
       <c r="B24" s="3">
         <v>6</v>
       </c>
-      <c r="C24" s="51"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="52"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="44"/>
       <c r="F24" s="3"/>
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
@@ -1189,9 +1193,9 @@
       <c r="B25" s="36">
         <v>7</v>
       </c>
-      <c r="C25" s="53"/>
-      <c r="D25" s="54"/>
-      <c r="E25" s="54"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
       <c r="F25" s="36"/>
     </row>
     <row r="26" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1228,41 +1232,44 @@
       </c>
     </row>
     <row r="28" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="49" t="s">
+      <c r="A28" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
+      <c r="B28" s="40"/>
+      <c r="C28" s="40"/>
       <c r="E28" t="s">
         <v>36</v>
       </c>
+      <c r="H28" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="29" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="49" t="s">
+      <c r="A29" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
       <c r="D29">
         <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="49" t="s">
+      <c r="A30" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="B30" s="37"/>
-      <c r="C30" s="37"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
       <c r="D30">
         <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="49" t="s">
+      <c r="A31" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="B31" s="37"/>
-      <c r="C31" s="37"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
       <c r="D31">
         <v>1</v>
       </c>
@@ -2238,21 +2245,29 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="J17:L17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="J10:L10"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="C10:E10"/>
@@ -2262,31 +2277,23 @@
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="C13:E13"/>
     <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="J17:L17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="C24:E24"/>
     <mergeCell ref="G22:H22"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="C21:E21"/>
     <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A31:C31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
portfolio website in progress
</commit_message>
<xml_diff>
--- a/Clyde_softskills/OKR framework IrenevDijk Q1.xlsx
+++ b/Clyde_softskills/OKR framework IrenevDijk Q1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/irene/Desktop/Techgrounds/NEW-TG-Web-development/Clyde_softskills/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A0916A-D264-BA4E-84CE-DE94914B9B5E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32549373-589D-274F-BD23-91BD5ECF1419}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="43">
   <si>
     <t>Timeframe</t>
   </si>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t>the subtle art of not giving a F</t>
+  </si>
+  <si>
+    <t>22.5%</t>
   </si>
 </sst>
 </file>
@@ -730,7 +733,7 @@
   <dimension ref="A1:M1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1004,8 +1007,8 @@
       </c>
       <c r="D13" s="40"/>
       <c r="E13" s="40"/>
-      <c r="F13" s="20">
-        <v>0.18</v>
+      <c r="F13" s="20" t="s">
+        <v>42</v>
       </c>
       <c r="G13" s="40"/>
       <c r="H13" s="40"/>
@@ -1027,7 +1030,7 @@
       <c r="D14" s="40"/>
       <c r="E14" s="40"/>
       <c r="F14" s="20">
-        <v>0.5</v>
+        <v>0.83</v>
       </c>
       <c r="G14" s="40"/>
       <c r="H14" s="40"/>
@@ -1298,6 +1301,9 @@
       <c r="I30">
         <v>1</v>
       </c>
+      <c r="K30">
+        <v>2</v>
+      </c>
     </row>
     <row r="31" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="39" t="s">
@@ -1315,7 +1321,10 @@
         <v>2</v>
       </c>
       <c r="J31">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="K31">
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
portfolio website versie 1 af
</commit_message>
<xml_diff>
--- a/Clyde_softskills/OKR framework IrenevDijk Q1.xlsx
+++ b/Clyde_softskills/OKR framework IrenevDijk Q1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/irene/Desktop/Techgrounds/NEW-TG-Web-development/Clyde_softskills/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32549373-589D-274F-BD23-91BD5ECF1419}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D5EBB0-2D47-D848-80C8-ABB484E0FFDF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -148,7 +148,7 @@
     <t>the subtle art of not giving a F</t>
   </si>
   <si>
-    <t>22.5%</t>
+    <t>0.5</t>
   </si>
 </sst>
 </file>
@@ -477,26 +477,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="11" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -510,8 +490,28 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="11" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -733,7 +733,7 @@
   <dimension ref="A1:M1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="G14" sqref="G14:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -770,25 +770,25 @@
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="50"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="38"/>
       <c r="E2" s="6"/>
       <c r="F2" s="7"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="50"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="38"/>
       <c r="J2" s="8"/>
       <c r="K2" s="9"/>
       <c r="L2" s="10"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="53"/>
-      <c r="B3" s="54"/>
-      <c r="C3" s="55" t="s">
+      <c r="A3" s="41"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="52"/>
-      <c r="E3" s="50"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="38"/>
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
       <c r="H3" s="12"/>
@@ -809,11 +809,11 @@
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
       <c r="I4" s="14"/>
-      <c r="J4" s="44" t="s">
+      <c r="J4" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="40"/>
-      <c r="L4" s="40"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="44"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
@@ -822,16 +822,16 @@
       <c r="B5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
       <c r="F5" s="16"/>
-      <c r="G5" s="41" t="s">
+      <c r="G5" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="40"/>
+      <c r="H5" s="44"/>
       <c r="I5" s="15" t="s">
         <v>13</v>
       </c>
@@ -852,16 +852,16 @@
       <c r="B6" s="19">
         <v>1</v>
       </c>
-      <c r="C6" s="39" t="s">
+      <c r="C6" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
       <c r="F6" s="20">
         <v>0.66</v>
       </c>
-      <c r="G6" s="48"/>
-      <c r="H6" s="40"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="44"/>
       <c r="I6" s="21" t="s">
         <v>16</v>
       </c>
@@ -874,14 +874,14 @@
       <c r="B7" s="19">
         <v>2</v>
       </c>
-      <c r="C7" s="46" t="s">
+      <c r="C7" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
       <c r="F7" s="24"/>
-      <c r="G7" s="48"/>
-      <c r="H7" s="40"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="44"/>
       <c r="I7" s="25"/>
       <c r="J7" s="22"/>
       <c r="K7" s="23"/>
@@ -892,14 +892,14 @@
       <c r="B8" s="19">
         <v>3</v>
       </c>
-      <c r="C8" s="57" t="s">
+      <c r="C8" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
       <c r="F8" s="24"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="40"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="44"/>
       <c r="I8" s="25"/>
       <c r="J8" s="22"/>
       <c r="K8" s="23"/>
@@ -910,14 +910,14 @@
       <c r="B9" s="19">
         <v>4</v>
       </c>
-      <c r="C9" s="57" t="s">
+      <c r="C9" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
       <c r="F9" s="24"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="40"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="44"/>
       <c r="I9" s="25"/>
       <c r="J9" s="22"/>
       <c r="K9" s="23"/>
@@ -930,18 +930,18 @@
       <c r="B10" s="19">
         <v>5</v>
       </c>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
       <c r="F10" s="24"/>
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
-      <c r="J10" s="45" t="s">
+      <c r="J10" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="K10" s="40"/>
-      <c r="L10" s="40"/>
+      <c r="K10" s="44"/>
+      <c r="L10" s="44"/>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="28" t="s">
@@ -950,16 +950,16 @@
       <c r="B11" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="41" t="s">
+      <c r="C11" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
       <c r="F11" s="29"/>
-      <c r="G11" s="41" t="s">
+      <c r="G11" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="40"/>
+      <c r="H11" s="44"/>
       <c r="I11" s="15" t="s">
         <v>13</v>
       </c>
@@ -980,16 +980,16 @@
       <c r="B12" s="19">
         <v>1</v>
       </c>
-      <c r="C12" s="39" t="s">
+      <c r="C12" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
       <c r="F12" s="20">
         <v>0.1</v>
       </c>
-      <c r="G12" s="40"/>
-      <c r="H12" s="40"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="44"/>
       <c r="I12" s="33" t="s">
         <v>20</v>
       </c>
@@ -1002,16 +1002,16 @@
       <c r="B13" s="19">
         <v>2</v>
       </c>
-      <c r="C13" s="39" t="s">
+      <c r="C13" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="20">
+        <v>0.32</v>
+      </c>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
       <c r="I13" s="33" t="s">
         <v>22</v>
       </c>
@@ -1024,16 +1024,16 @@
       <c r="B14" s="19">
         <v>3</v>
       </c>
-      <c r="C14" s="39" t="s">
+      <c r="C14" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
       <c r="F14" s="20">
         <v>0.83</v>
       </c>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
       <c r="I14" s="33" t="s">
         <v>24</v>
       </c>
@@ -1046,12 +1046,12 @@
       <c r="B15" s="19">
         <v>4</v>
       </c>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
       <c r="F15" s="24"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
       <c r="I15" s="25"/>
       <c r="J15" s="23"/>
       <c r="K15" s="23"/>
@@ -1062,12 +1062,12 @@
       <c r="B16" s="19">
         <v>5</v>
       </c>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
       <c r="F16" s="24"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
       <c r="I16" s="25"/>
       <c r="J16" s="23"/>
       <c r="K16" s="23"/>
@@ -1078,18 +1078,18 @@
       <c r="B17" s="3">
         <v>6</v>
       </c>
-      <c r="C17" s="42"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="43"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="55"/>
       <c r="F17" s="3"/>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
-      <c r="J17" s="44" t="s">
+      <c r="J17" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="K17" s="40"/>
-      <c r="L17" s="40"/>
+      <c r="K17" s="44"/>
+      <c r="L17" s="44"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
@@ -1098,16 +1098,16 @@
       <c r="B18" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="56" t="s">
+      <c r="C18" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="44"/>
       <c r="F18" s="34"/>
-      <c r="G18" s="41" t="s">
+      <c r="G18" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="H18" s="40"/>
+      <c r="H18" s="44"/>
       <c r="I18" s="15" t="s">
         <v>13</v>
       </c>
@@ -1126,12 +1126,12 @@
       <c r="B19" s="19">
         <v>1</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
       <c r="F19" s="24"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="44"/>
       <c r="I19" s="25"/>
       <c r="J19" s="23"/>
       <c r="K19" s="23"/>
@@ -1142,12 +1142,12 @@
       <c r="B20" s="19">
         <v>2</v>
       </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
       <c r="F20" s="24"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="40"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="44"/>
       <c r="I20" s="25"/>
       <c r="J20" s="23"/>
       <c r="K20" s="23"/>
@@ -1158,12 +1158,12 @@
       <c r="B21" s="19">
         <v>3</v>
       </c>
-      <c r="C21" s="40"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="44"/>
       <c r="F21" s="24"/>
-      <c r="G21" s="40"/>
-      <c r="H21" s="40"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="44"/>
       <c r="I21" s="25"/>
       <c r="J21" s="23"/>
       <c r="K21" s="23"/>
@@ -1174,12 +1174,12 @@
       <c r="B22" s="19">
         <v>4</v>
       </c>
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="44"/>
       <c r="F22" s="24"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="40"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="44"/>
       <c r="I22" s="25"/>
       <c r="J22" s="23"/>
       <c r="K22" s="23"/>
@@ -1190,12 +1190,12 @@
       <c r="B23" s="19">
         <v>5</v>
       </c>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
       <c r="F23" s="24"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="40"/>
+      <c r="G23" s="44"/>
+      <c r="H23" s="44"/>
       <c r="I23" s="25"/>
       <c r="J23" s="23"/>
       <c r="K23" s="23"/>
@@ -1206,9 +1206,9 @@
       <c r="B24" s="3">
         <v>6</v>
       </c>
-      <c r="C24" s="42"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="43"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="55"/>
       <c r="F24" s="3"/>
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
@@ -1222,9 +1222,9 @@
       <c r="B25" s="36">
         <v>7</v>
       </c>
-      <c r="C25" s="37"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="38"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="57"/>
       <c r="F25" s="36"/>
     </row>
     <row r="26" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1261,11 +1261,11 @@
       </c>
     </row>
     <row r="28" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="39" t="s">
+      <c r="A28" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="40"/>
-      <c r="C28" s="40"/>
+      <c r="B28" s="44"/>
+      <c r="C28" s="44"/>
       <c r="E28" t="s">
         <v>36</v>
       </c>
@@ -1277,21 +1277,21 @@
       </c>
     </row>
     <row r="29" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
       <c r="D29">
         <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
+      <c r="B30" s="44"/>
+      <c r="C30" s="44"/>
       <c r="D30">
         <v>5</v>
       </c>
@@ -1302,15 +1302,18 @@
         <v>1</v>
       </c>
       <c r="K30">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="L30" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="39" t="s">
+      <c r="A31" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="B31" s="40"/>
-      <c r="C31" s="40"/>
+      <c r="B31" s="44"/>
+      <c r="C31" s="44"/>
       <c r="D31">
         <v>1</v>
       </c>
@@ -2298,6 +2301,39 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="49">
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="J17:L17"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="A3:B3"/>
@@ -2314,39 +2350,6 @@
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="G9:H9"/>
     <mergeCell ref="C15:E15"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="J17:L17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A31:C31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>